<commit_message>
Majority of match scorecards by over and bowlers done. Points table work half done.
</commit_message>
<xml_diff>
--- a/schema.xlsx
+++ b/schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\pythonPractice\big projects\IPL Analytics\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\pythonPractice\big projects\IPL Analytics\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED70B4A6-2AF7-418E-B131-F8B90931F8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D38745-0473-447A-9604-742ABE266EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="143">
   <si>
     <t>matches</t>
   </si>
@@ -114,24 +114,6 @@
     <t>views</t>
   </si>
   <si>
-    <t>group phase matches</t>
-  </si>
-  <si>
-    <t>playoff matches</t>
-  </si>
-  <si>
-    <t>finals matches</t>
-  </si>
-  <si>
-    <t>super over ball by ball</t>
-  </si>
-  <si>
-    <t>record</t>
-  </si>
-  <si>
-    <t>table rank</t>
-  </si>
-  <si>
     <t>for_runs</t>
   </si>
   <si>
@@ -141,9 +123,6 @@
     <t>for_overs</t>
   </si>
   <si>
-    <t>rank</t>
-  </si>
-  <si>
     <t>net_run_rate</t>
   </si>
   <si>
@@ -195,9 +174,6 @@
     <t>bowling_hand</t>
   </si>
   <si>
-    <t>match_scorecard</t>
-  </si>
-  <si>
     <t>inning</t>
   </si>
   <si>
@@ -246,9 +222,6 @@
     <t>doubles_taken</t>
   </si>
   <si>
-    <t>runs_scored_in_final_4 overs</t>
-  </si>
-  <si>
     <t>batting_team</t>
   </si>
   <si>
@@ -303,27 +276,6 @@
     <t>4_scored</t>
   </si>
   <si>
-    <t>batting_stats_playoffs</t>
-  </si>
-  <si>
-    <t>batting_stats_group_stage</t>
-  </si>
-  <si>
-    <t>home_points</t>
-  </si>
-  <si>
-    <t>away_points</t>
-  </si>
-  <si>
-    <t>wins</t>
-  </si>
-  <si>
-    <t>losses</t>
-  </si>
-  <si>
-    <t>no_results</t>
-  </si>
-  <si>
     <t>tosses_won</t>
   </si>
   <si>
@@ -360,15 +312,6 @@
     <t>batsman_runs_on_other_end</t>
   </si>
   <si>
-    <t>batsman_balls_on_other_end</t>
-  </si>
-  <si>
-    <t>total_runs_scored</t>
-  </si>
-  <si>
-    <t>total_wickets_fallen</t>
-  </si>
-  <si>
     <t>potm</t>
   </si>
   <si>
@@ -399,16 +342,118 @@
     <t>stadium</t>
   </si>
   <si>
-    <t>match_scorecard_by_over</t>
-  </si>
-  <si>
     <t>runs</t>
   </si>
   <si>
     <t>wickets</t>
   </si>
   <si>
-    <t>extras_conceded</t>
+    <t>balls</t>
+  </si>
+  <si>
+    <t>singles</t>
+  </si>
+  <si>
+    <t>doubles</t>
+  </si>
+  <si>
+    <t>ball_on_dismissal</t>
+  </si>
+  <si>
+    <t>ball_on_arrival</t>
+  </si>
+  <si>
+    <t>partner_batsman_balls</t>
+  </si>
+  <si>
+    <t>matches_type</t>
+  </si>
+  <si>
+    <t>runs_in_powerplay</t>
+  </si>
+  <si>
+    <t>runs_in_end</t>
+  </si>
+  <si>
+    <t>dinda_academy</t>
+  </si>
+  <si>
+    <t>player_points_match</t>
+  </si>
+  <si>
+    <t>team_performance</t>
+  </si>
+  <si>
+    <t>match_over_scorecards</t>
+  </si>
+  <si>
+    <t>match_batsman_scorecard</t>
+  </si>
+  <si>
+    <t>home_wins</t>
+  </si>
+  <si>
+    <t>away_losses</t>
+  </si>
+  <si>
+    <t>record (string)</t>
+  </si>
+  <si>
+    <t>away_wins</t>
+  </si>
+  <si>
+    <t>home_losses</t>
+  </si>
+  <si>
+    <t>home_no_results</t>
+  </si>
+  <si>
+    <t>away_no_results</t>
+  </si>
+  <si>
+    <t>batting_stats</t>
+  </si>
+  <si>
+    <t>bowler_stats</t>
+  </si>
+  <si>
+    <t>sixes</t>
+  </si>
+  <si>
+    <t>fours</t>
+  </si>
+  <si>
+    <t>extras</t>
+  </si>
+  <si>
+    <t>match_bowler_scorecards</t>
+  </si>
+  <si>
+    <t>overs</t>
+  </si>
+  <si>
+    <t>bowled</t>
+  </si>
+  <si>
+    <t>caught</t>
+  </si>
+  <si>
+    <t>lbw</t>
+  </si>
+  <si>
+    <t>stumped</t>
+  </si>
+  <si>
+    <t>maidens</t>
+  </si>
+  <si>
+    <t>hattricks</t>
+  </si>
+  <si>
+    <t>wicketkeeper_stats</t>
+  </si>
+  <si>
+    <t>fielding_stats</t>
   </si>
 </sst>
 </file>
@@ -457,12 +502,13 @@
     <font>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -502,7 +548,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -788,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,19 +847,19 @@
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -820,23 +868,23 @@
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" t="s">
-        <v>56</v>
+      <c r="G2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
+        <v>128</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -856,19 +904,16 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -876,31 +921,28 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
         <v>7</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -908,31 +950,28 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -940,31 +979,28 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>44</v>
+      <c r="F7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="J7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -972,31 +1008,28 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
+        <v>99</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1004,28 +1037,28 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" t="s">
-        <v>34</v>
+      <c r="F9" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="I9" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="J9" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1033,31 +1066,28 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>35</v>
+      <c r="F10" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="I10" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="J10" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1065,28 +1095,28 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1094,31 +1124,28 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="J12" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1126,28 +1153,28 @@
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="J13" t="s">
-        <v>72</v>
-      </c>
-      <c r="K13" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1155,28 +1182,28 @@
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="G14" t="s">
+        <v>110</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" t="s">
-        <v>72</v>
+        <v>51</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="J14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K14" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1184,31 +1211,28 @@
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>111</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="J15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K15" t="s">
-        <v>125</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1216,292 +1240,357 @@
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>60</v>
+        <v>132</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
-      </c>
-      <c r="K16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" t="s">
-        <v>104</v>
-      </c>
-      <c r="K17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J18" t="s">
-        <v>105</v>
-      </c>
-      <c r="K18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="G19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" t="s">
-        <v>66</v>
+        <v>108</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="J19" t="s">
-        <v>106</v>
-      </c>
-      <c r="K19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>99</v>
+      <c r="F20" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" t="s">
-        <v>67</v>
+        <v>109</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="J20" t="s">
-        <v>107</v>
-      </c>
-      <c r="K20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>111</v>
+        <v>85</v>
+      </c>
+      <c r="G21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="J21" t="s">
-        <v>108</v>
-      </c>
-      <c r="K21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" t="s">
+        <v>131</v>
+      </c>
+      <c r="J22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="6"/>
+      <c r="F23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="6"/>
+      <c r="F24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" s="3" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H23" t="s">
-        <v>123</v>
-      </c>
-      <c r="J23" t="s">
-        <v>114</v>
-      </c>
-      <c r="K23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="K24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added python script (with most steps defined and dotenv support) for most intricate formatting. Initialized final analytics script. Improved schema and match_bowler_scorecards
</commit_message>
<xml_diff>
--- a/schema.xlsx
+++ b/schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\pythonPractice\big projects\IPL Analytics\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D38745-0473-447A-9604-742ABE266EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1055AF-5753-496D-9E23-901D4703BDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="151">
   <si>
     <t>matches</t>
   </si>
@@ -309,9 +309,6 @@
     <t>wage</t>
   </si>
   <si>
-    <t>batsman_runs_on_other_end</t>
-  </si>
-  <si>
     <t>potm</t>
   </si>
   <si>
@@ -357,15 +354,6 @@
     <t>doubles</t>
   </si>
   <si>
-    <t>ball_on_dismissal</t>
-  </si>
-  <si>
-    <t>ball_on_arrival</t>
-  </si>
-  <si>
-    <t>partner_batsman_balls</t>
-  </si>
-  <si>
     <t>matches_type</t>
   </si>
   <si>
@@ -454,13 +442,49 @@
   </si>
   <si>
     <t>fielding_stats</t>
+  </si>
+  <si>
+    <t>overs_on_arrival</t>
+  </si>
+  <si>
+    <t>overs_on_dismissal</t>
+  </si>
+  <si>
+    <t>end_partner_runs</t>
+  </si>
+  <si>
+    <t>end_partner_balls</t>
+  </si>
+  <si>
+    <t>runs_conceded</t>
+  </si>
+  <si>
+    <t>dots</t>
+  </si>
+  <si>
+    <t>striker_runs</t>
+  </si>
+  <si>
+    <t>striker_balls</t>
+  </si>
+  <si>
+    <t>non_striker_runs</t>
+  </si>
+  <si>
+    <t>non_striker_balls</t>
+  </si>
+  <si>
+    <t>team_runs</t>
+  </si>
+  <si>
+    <t>team_overs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,6 +540,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -537,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -554,6 +586,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,19 +905,19 @@
         <v>2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -930,7 +963,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
         <v>49</v>
@@ -959,7 +992,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G6" t="s">
         <v>55</v>
@@ -968,7 +1001,7 @@
         <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
       <c r="J6" t="s">
         <v>56</v>
@@ -988,16 +1021,16 @@
         <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G7" t="s">
         <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J7" t="s">
         <v>61</v>
@@ -1011,22 +1044,22 @@
         <v>58</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" t="s">
         <v>105</v>
       </c>
-      <c r="H8" t="s">
-        <v>106</v>
-      </c>
-      <c r="I8" t="s">
-        <v>106</v>
+      <c r="I8" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="J8" t="s">
         <v>60</v>
@@ -1040,22 +1073,22 @@
         <v>59</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" t="s">
         <v>126</v>
       </c>
-      <c r="G9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H9" t="s">
-        <v>130</v>
-      </c>
       <c r="I9" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="J9" t="s">
         <v>81</v>
@@ -1069,22 +1102,22 @@
         <v>67</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G10" t="s">
         <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I10" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="J10" t="s">
         <v>82</v>
@@ -1098,13 +1131,13 @@
         <v>68</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
@@ -1113,7 +1146,7 @@
         <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
       <c r="J11" t="s">
         <v>62</v>
@@ -1127,10 +1160,10 @@
         <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
         <v>29</v>
@@ -1139,10 +1172,10 @@
         <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="J12" t="s">
         <v>63</v>
@@ -1156,10 +1189,10 @@
         <v>69</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13" t="s">
         <v>30</v>
@@ -1168,10 +1201,10 @@
         <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J13" t="s">
         <v>64</v>
@@ -1185,22 +1218,22 @@
         <v>70</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" t="s">
         <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="H14" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>70</v>
+      <c r="I14" t="s">
+        <v>126</v>
       </c>
       <c r="J14" t="s">
         <v>51</v>
@@ -1214,7 +1247,7 @@
         <v>71</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
@@ -1223,13 +1256,13 @@
         <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="H15" t="s">
         <v>53</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>73</v>
+      <c r="I15" t="s">
+        <v>128</v>
       </c>
       <c r="J15" t="s">
         <v>50</v>
@@ -1243,7 +1276,7 @@
         <v>72</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>23</v>
@@ -1252,16 +1285,16 @@
         <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="H16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="J16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1272,7 +1305,7 @@
         <v>73</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>22</v>
@@ -1281,16 +1314,16 @@
         <v>35</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>70</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>136</v>
+        <v>73</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1301,7 +1334,7 @@
         <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>24</v>
@@ -1315,11 +1348,11 @@
       <c r="H18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>137</v>
+      <c r="I18" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1327,7 +1360,7 @@
         <v>75</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>25</v>
@@ -1336,13 +1369,13 @@
         <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>138</v>
+      <c r="I19" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="J19" t="s">
         <v>88</v>
@@ -1354,7 +1387,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>26</v>
@@ -1363,13 +1396,13 @@
         <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>139</v>
+      <c r="I20" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="J20" t="s">
         <v>89</v>
@@ -1381,7 +1414,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>27</v>
@@ -1394,6 +1427,9 @@
       </c>
       <c r="H21" s="3" t="s">
         <v>74</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="J21" t="s">
         <v>90</v>
@@ -1404,8 +1440,8 @@
         <v>78</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="3" t="s">
-        <v>80</v>
+      <c r="D22" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -1414,7 +1450,10 @@
         <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="J22" t="s">
         <v>91</v>
@@ -1425,12 +1464,14 @@
         <v>79</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="F23" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J23" t="s">
         <v>92</v>
@@ -1441,33 +1482,44 @@
         <v>80</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="F24" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
+      <c r="D25" s="6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
+      <c r="D26" s="6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" t="s">
-        <v>5</v>
+      <c r="D27" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1478,119 +1530,119 @@
         <v>87</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" t="s">
-        <v>39</v>
-      </c>
       <c r="E29" t="s">
         <v>40</v>
       </c>
       <c r="F29" t="s">
         <v>36</v>
       </c>
+      <c r="G29" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" t="s">
-        <v>44</v>
-      </c>
       <c r="E30" t="s">
         <v>41</v>
       </c>
       <c r="F30" t="s">
         <v>38</v>
       </c>
+      <c r="G30" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" t="s">
-        <v>38</v>
-      </c>
       <c r="E31" t="s">
         <v>42</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
       </c>
+      <c r="G31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E32" t="s">
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" t="s">
+      <c r="E33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" t="s">
+      <c r="E34" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="3" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="E35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+      <c r="E36" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>142</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C36" s="2"/>
-      <c r="D36" t="s">
+      <c r="G36" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
-      <c r="D37" t="s">
+      <c r="G37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
     </row>
   </sheetData>

</xml_diff>